<commit_message>
Take first look at simulation data
</commit_message>
<xml_diff>
--- a/data/dfd01.xlsx
+++ b/data/dfd01.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="74">
   <si>
     <t xml:space="preserve">node</t>
   </si>
@@ -41,7 +41,10 @@
     <t xml:space="preserve">domain</t>
   </si>
   <si>
-    <t xml:space="preserve">range</t>
+    <t xml:space="preserve">range_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">range_max</t>
   </si>
   <si>
     <t xml:space="preserve">value_resolution</t>
@@ -62,15 +65,27 @@
     <t xml:space="preserve">parameter</t>
   </si>
   <si>
+    <t xml:space="preserve">error weight</t>
+  </si>
+  <si>
     <t xml:space="preserve">FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">real</t>
   </si>
   <si>
+    <t xml:space="preserve">Fixed parameter. Range assumed</t>
+  </si>
+  <si>
     <t xml:space="preserve">k_i</t>
   </si>
   <si>
+    <t xml:space="preserve">integrated error weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed parameter. Range assumed. This interacts with k_windup and k_p, and is not necessarily the nicest parameterisation.</t>
+  </si>
+  <si>
     <t xml:space="preserve">k_tgt</t>
   </si>
   <si>
@@ -80,6 +95,9 @@
     <t xml:space="preserve">k_windup</t>
   </si>
   <si>
+    <t xml:space="preserve">integrated error limit</t>
+  </si>
+  <si>
     <t xml:space="preserve">z</t>
   </si>
   <si>
@@ -89,6 +107,9 @@
     <t xml:space="preserve">altitude</t>
   </si>
   <si>
+    <t xml:space="preserve">Range assumed as reasonable altitudes for holding</t>
+  </si>
+  <si>
     <t xml:space="preserve">dz</t>
   </si>
   <si>
@@ -101,7 +122,7 @@
     <t xml:space="preserve">output</t>
   </si>
   <si>
-    <t xml:space="preserve">motor command</t>
+    <t xml:space="preserve">motor demand</t>
   </si>
   <si>
     <t xml:space="preserve">e</t>
@@ -113,22 +134,28 @@
     <t xml:space="preserve">vertical error</t>
   </si>
   <si>
-    <t xml:space="preserve">ei_t</t>
+    <t xml:space="preserve">ei</t>
   </si>
   <si>
     <t xml:space="preserve">error integral @ t</t>
   </si>
   <si>
-    <t xml:space="preserve">Default is initial value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ei_t1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ei_t-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">error integral @ t-1</t>
+    <t xml:space="preserve">Default is initial value. Range is imposed by k_windup.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lag (i9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lag(ei)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is identical to ei lagged by one time step.</t>
   </si>
   <si>
     <t xml:space="preserve">i1</t>
@@ -137,9 +164,6 @@
     <t xml:space="preserve">- (I1)</t>
   </si>
   <si>
-    <t xml:space="preserve">function</t>
-  </si>
-  <si>
     <t xml:space="preserve">k_tgt – z</t>
   </si>
   <si>
@@ -170,6 +194,9 @@
     <t xml:space="preserve">e + ei_t-1</t>
   </si>
   <si>
+    <t xml:space="preserve">Range depends on k_windup</t>
+  </si>
+  <si>
     <t xml:space="preserve">i5</t>
   </si>
   <si>
@@ -185,7 +212,7 @@
     <t xml:space="preserve">* (i6)</t>
   </si>
   <si>
-    <t xml:space="preserve">k_i * i5</t>
+    <t xml:space="preserve">k_i * ei_t</t>
   </si>
   <si>
     <t xml:space="preserve">i7</t>
@@ -197,19 +224,35 @@
     <t xml:space="preserve">I3 * i6</t>
   </si>
   <si>
+    <t xml:space="preserve">i8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clip (i8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constrain(i7, 0, 1)</t>
+  </si>
+  <si>
     <t xml:space="preserve">from</t>
   </si>
   <si>
     <t xml:space="preserve">to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -283,7 +326,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -296,6 +339,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -304,11 +351,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -329,13 +384,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13:C15"/>
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.69"/>
@@ -343,395 +398,666 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="8.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="50.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0.001</v>
       </c>
       <c r="J2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="n">
         <v>0.2</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0.001</v>
       </c>
       <c r="J3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3" t="n">
         <v>3</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="L4" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.001</v>
       </c>
       <c r="J5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3" t="n">
         <v>0.2</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>14</v>
+      <c r="I6" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0.001</v>
       </c>
       <c r="J10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K10" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>35</v>
+      <c r="L10" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="7" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="9"/>
+      <c r="L11" s="7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="D13" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="E13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>38</v>
+        <v>52</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>38</v>
+        <v>55</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>-10</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>38</v>
+        <v>62</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>-25</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>38</v>
+        <v>65</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>-30</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -750,224 +1076,251 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="1" sqref="C13:C15 G22"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.59"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>59</v>
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>45</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>45</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>48</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>48</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>51</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>51</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>54</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>54</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>40</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>37</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>58</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>13</v>
+        <v>58</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>61</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>13</v>
+        <v>61</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>13</v>
+        <v>64</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>13</v>
+        <v>64</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>13</v>
+        <v>67</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete investigation of simulation data
</commit_message>
<xml_diff>
--- a/data/dfd01.xlsx
+++ b/data/dfd01.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="76">
   <si>
     <t xml:space="preserve">node</t>
   </si>
@@ -119,117 +119,117 @@
     <t xml:space="preserve">u</t>
   </si>
   <si>
+    <t xml:space="preserve">reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motor demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vertical error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error integral @ t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default is initial value. Range is imposed by k_windup.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lag (i9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lag(ei)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is identical to ei lagged by one time step.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- (I1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_tgt – z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- (i2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(k_tgt – z) – dz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* (i3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_p * e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ (i4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e + ei_t-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Range depends on k_windup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clip (i5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constrain(ei_t, k_windup)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* (i6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_i * ei_t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ (i7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I3 * i6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clip (i8)</t>
+  </si>
+  <si>
     <t xml:space="preserve">output</t>
   </si>
   <si>
-    <t xml:space="preserve">motor demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">internal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vertical error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ei</t>
-  </si>
-  <si>
-    <t xml:space="preserve">error integral @ t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default is initial value. Range is imposed by k_windup.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lag (i9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lag(ei)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is identical to ei lagged by one time step.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- (I1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_tgt – z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- (i2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(k_tgt – z) – dz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* (i3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_p * e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ (i4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e + ei_t-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Range depends on k_windup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clip (i5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constrain(ei_t, k_windup)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* (i6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_i * ei_t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ (i7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I3 * i6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clip (i8)</t>
-  </si>
-  <si>
     <t xml:space="preserve">constrain(i7, 0, 1)</t>
   </si>
   <si>
@@ -243,6 +243,12 @@
   </si>
   <si>
     <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equality to import</t>
   </si>
 </sst>
 </file>
@@ -387,10 +393,10 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="14:14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.69"/>
@@ -703,11 +709,11 @@
         <v>34</v>
       </c>
       <c r="C9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="E9" s="2" t="s">
         <v>15</v>
       </c>
@@ -715,10 +721,10 @@
         <v>16</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>-5</v>
+        <v>-25</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>0.001</v>
@@ -729,16 +735,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>15</v>
@@ -762,22 +768,22 @@
         <v>0</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="E11" s="2" t="s">
         <v>15</v>
       </c>
@@ -785,10 +791,10 @@
         <v>16</v>
       </c>
       <c r="G11" s="7" t="n">
-        <v>-0.2</v>
+        <v>-1</v>
       </c>
       <c r="H11" s="7" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>0.001</v>
@@ -798,22 +804,22 @@
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="E12" s="2" t="s">
         <v>15</v>
       </c>
@@ -821,10 +827,10 @@
         <v>16</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>-5</v>
+        <v>-20</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>0.001</v>
@@ -835,17 +841,17 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
@@ -853,10 +859,10 @@
         <v>16</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>-5</v>
+        <v>-25</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>0.001</v>
@@ -867,17 +873,17 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
@@ -885,10 +891,10 @@
         <v>16</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>-5</v>
+        <v>-25</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>0.001</v>
@@ -899,52 +905,52 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="0" t="s">
+      <c r="E15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>-26</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <v>-10</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L15" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
@@ -952,10 +958,10 @@
         <v>16</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>0.001</v>
@@ -966,17 +972,17 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>63</v>
-      </c>
       <c r="E17" s="2" t="s">
         <v>15</v>
       </c>
@@ -984,10 +990,10 @@
         <v>16</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>-25</v>
+        <v>-5</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>0.001</v>
@@ -998,16 +1004,16 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>66</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>15</v>
@@ -1030,13 +1036,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>69</v>
@@ -1076,13 +1082,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="14:14 E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.59"/>
@@ -1101,13 +1107,16 @@
       <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>72</v>
@@ -1121,7 +1130,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>73</v>
@@ -1132,10 +1141,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>72</v>
@@ -1149,7 +1158,7 @@
         <v>29</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>73</v>
@@ -1160,21 +1169,27 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="C6" s="0" t="s">
+        <v>74</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>15</v>
@@ -1182,10 +1197,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
@@ -1193,10 +1208,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>15</v>
@@ -1204,10 +1219,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>15</v>
@@ -1215,10 +1230,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>15</v>
@@ -1226,10 +1241,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>15</v>
@@ -1237,21 +1252,27 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>58</v>
+        <v>36</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>74</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>15</v>
@@ -1259,10 +1280,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>15</v>
@@ -1273,7 +1294,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>15</v>
@@ -1281,10 +1302,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>15</v>
@@ -1292,10 +1313,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>15</v>
@@ -1303,10 +1324,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>15</v>
@@ -1314,13 +1335,19 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="C20" s="0" t="s">
+        <v>74</v>
+      </c>
       <c r="D20" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add multi target simulation data
</commit_message>
<xml_diff>
--- a/data/dfd01.xlsx
+++ b/data/dfd01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="78">
   <si>
     <t xml:space="preserve">node</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t xml:space="preserve">equality to import</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equality to import (if u_clip = TRUE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equality to import (if u_clip = FALSE)</t>
   </si>
 </sst>
 </file>
@@ -392,11 +398,11 @@
   </sheetPr>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="14:14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.69"/>
@@ -405,7 +411,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="8.14"/>
@@ -1082,13 +1087,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="14:14 E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.59"/>
@@ -1347,7 +1352,24 @@
         <v>15</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>